<commit_message>
Added files for testing, Added code and notes
</commit_message>
<xml_diff>
--- a/images/Other_Files/TblTestBook.xlsx
+++ b/images/Other_Files/TblTestBook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/749995370292dc61/Documents/Coding Stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\Posts\images\Other_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB05264A-D839-4D51-B323-D0DDE97269AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD5A61-9AAE-4DEF-B258-4F79F4D5A88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="504" windowWidth="17280" windowHeight="8880" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
+    <workbookView xWindow="96" yWindow="1920" windowWidth="22944" windowHeight="10164" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arb_Tbl" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>myHead1</t>
   </si>
@@ -62,16 +63,106 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Attr1</t>
+  </si>
+  <si>
+    <t>Attr2</t>
+  </si>
+  <si>
+    <t>Attr3</t>
+  </si>
+  <si>
+    <t>Attr4</t>
+  </si>
+  <si>
+    <t>Attr5</t>
+  </si>
+  <si>
+    <t>Attr6</t>
+  </si>
+  <si>
+    <t>Attr7</t>
+  </si>
+  <si>
+    <t>Bob Back</t>
+  </si>
+  <si>
+    <t>Jeff Jahl</t>
+  </si>
+  <si>
+    <t>Hodge Hoss</t>
+  </si>
+  <si>
+    <t>Kev Kroll</t>
+  </si>
+  <si>
+    <t>Tim Tin</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Dick</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Blaire</t>
+  </si>
+  <si>
+    <t>Chuck</t>
+  </si>
+  <si>
+    <t>Darryl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,6 +216,39 @@
     <tableColumn id="3" xr3:uid="{362F9B8F-D43C-4334-BCAE-4AA090005C82}" name="myHead3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A788979B-9964-4770-A54C-0E42D2C70189}" name="tblHrs" displayName="tblHrs" ref="G13:H17">
+  <autoFilter ref="G13:H17" xr:uid="{A788979B-9964-4770-A54C-0E42D2C70189}"/>
+  <tableColumns count="2">
+    <tableColumn id="5" xr3:uid="{59BD9C4F-B49D-4CDA-A8DA-3BBD8F084EDE}" name="Names"/>
+    <tableColumn id="6" xr3:uid="{7999A9FA-87C2-4FFE-B573-F6184FEF03F1}" name="Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6CEC1EB2-AB48-4B56-B836-2EB5C6433F68}" name="tblHrs2" displayName="tblHrs2" ref="G7:H11">
+  <autoFilter ref="G7:H11" xr:uid="{6CEC1EB2-AB48-4B56-B836-2EB5C6433F68}"/>
+  <tableColumns count="2">
+    <tableColumn id="5" xr3:uid="{C79DE68B-A49B-43EE-AC2A-9EF527009BD3}" name="Names"/>
+    <tableColumn id="6" xr3:uid="{7C3501C7-2155-4518-B622-9DC010C28539}" name="Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E1F17F3-389C-42CE-9D90-859DC27E5C33}" name="tblHrs3" displayName="tblHrs3" ref="C18:D22">
+  <autoFilter ref="C18:D22" xr:uid="{9E1F17F3-389C-42CE-9D90-859DC27E5C33}"/>
+  <tableColumns count="2">
+    <tableColumn id="5" xr3:uid="{7B34FB1F-EEF5-4440-AB96-761BDB40B7B1}" name="Names"/>
+    <tableColumn id="6" xr3:uid="{D35E76F1-0FA6-42A0-80B3-8AC4B75BCA04}" name="Hours"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
@@ -425,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD34CBD-62ED-44F4-8AFC-CADDED702CE0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +560,7 @@
     <col min="1" max="3" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -458,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -469,7 +593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -480,10 +604,358 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E898CF44-CB42-49BE-BB13-B57007476583}">
+  <dimension ref="A3:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f ca="1">RAND()*5</f>
+        <v>4.6990756735648347</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:I8" ca="1" si="0">RAND()*5</f>
+        <v>4.6795048050815886</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46529949650559399</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8385221248428403</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9009454246757942</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0627777879519789</v>
+      </c>
+      <c r="I4">
+        <f ca="1">RAND()*5</f>
+        <v>3.6984916848324239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C8" ca="1" si="1">RAND()*5</f>
+        <v>4.560881689319551</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33022224740733463</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.3273282355194436</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8529113875815422</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5913561451086071</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5492039592550872</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.3242951987270137E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1150397738859819</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8595233109623468</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8423575068555493</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1603899131948028</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71922377686600536</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.3335723546263276</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27749126626764486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.3732597556838591</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3180400802021284</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94635213621455716</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5318828772723827</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2013453004101804</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73882087156698084</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1308919096502787</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6902311335181284E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.1080715424936409</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6576522448441389</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1313877453876002</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0989865257423528</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0796194145020257</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1509058708517639</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit to exmpl book
</commit_message>
<xml_diff>
--- a/images/Other_Files/TblTestBook.xlsx
+++ b/images/Other_Files/TblTestBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\Posts\images\Other_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD5A61-9AAE-4DEF-B258-4F79F4D5A88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CD44E0-9B5F-4ADE-A97D-96587582CC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="1920" windowWidth="22944" windowHeight="10164" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
+    <workbookView xWindow="312" yWindow="1620" windowWidth="12948" windowHeight="10164" activeTab="1" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD34CBD-62ED-44F4-8AFC-CADDED702CE0}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E898CF44-CB42-49BE-BB13-B57007476583}">
   <dimension ref="A3:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,31 +783,31 @@
       </c>
       <c r="C4">
         <f ca="1">RAND()*5</f>
-        <v>4.6990756735648347</v>
+        <v>0.75128259450252033</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:I8" ca="1" si="0">RAND()*5</f>
-        <v>4.6795048050815886</v>
+        <v>4.4204656384831917</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46529949650559399</v>
+        <v>3.938915873720541</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8385221248428403</v>
+        <v>4.8898980278003359</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9009454246757942</v>
+        <v>4.8630616178285067</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0627777879519789</v>
+        <v>4.447030945125011</v>
       </c>
       <c r="I4">
         <f ca="1">RAND()*5</f>
-        <v>3.6984916848324239</v>
+        <v>1.2195658937662452</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -819,31 +819,31 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C8" ca="1" si="1">RAND()*5</f>
-        <v>4.560881689319551</v>
+        <v>4.086109774231808</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33022224740733463</v>
+        <v>0.51889482867823022</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3273282355194436</v>
+        <v>1.1948241224480545</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8529113875815422</v>
+        <v>1.4546602344675859</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5913561451086071</v>
+        <v>8.8997254770577516E-2</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5492039592550872</v>
+        <v>4.9269143040358623</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3242951987270137E-2</v>
+        <v>0.76472455759957869</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -855,31 +855,31 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1150397738859819</v>
+        <v>0.10843562511844262</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8595233109623468</v>
+        <v>1.5664972624555495</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8423575068555493</v>
+        <v>2.3895875264151156</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1603899131948028</v>
+        <v>4.343378396384133</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71922377686600536</v>
+        <v>4.1264836303168559</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3335723546263276</v>
+        <v>4.6380897888060071</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27749126626764486</v>
+        <v>3.0099358268514402</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -891,31 +891,31 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3732597556838591</v>
+        <v>1.6428651209505425</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3180400802021284</v>
+        <v>0.9242720115923958</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94635213621455716</v>
+        <v>1.5600541635833238</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5318828772723827</v>
+        <v>1.0272119468846004</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2013453004101804</v>
+        <v>1.4286970049646226</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73882087156698084</v>
+        <v>3.2448431803146676</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1308919096502787</v>
+        <v>4.0873580361466457</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -927,31 +927,31 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6902311335181284E-2</v>
+        <v>2.3626575986660523</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1080715424936409</v>
+        <v>0.10651384847641832</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6576522448441389</v>
+        <v>4.1969840271567609</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1313877453876002</v>
+        <v>4.066367212268136</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0989865257423528</v>
+        <v>2.266040947090024</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0796194145020257</v>
+        <v>1.8839206858436142</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1509058708517639</v>
+        <v>4.4505516888358079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>